<commit_message>
Update KpiAgent related files
</commit_message>
<xml_diff>
--- a/Java code references - 21'04.xlsx
+++ b/Java code references - 21'04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C57D3AF-C137-4C5B-AB40-79EAAB4F53DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37FDDCF-0F34-4B0F-A0BC-6B1A8B1F44B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="144" windowWidth="22488" windowHeight="11808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="22488" windowHeight="11808" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref. Site" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="97">
   <si>
     <t>Type</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2541,6 +2541,63 @@
   </si>
   <si>
     <t>Convert Java object to JSON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What is a serialVersionUID and why should I use it?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- https://stackoverflow.com/questions/285793/what-is-a-serialversionuid-and-why-should-i-use-it</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SerialVersion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring JDBC
+Last modified: February 20, 2021
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- https://www.baeldung.com/spring-jdbc-jdbctemplate
+- 6.1. Basic Batch Operations Using JdbcTemplate
+Using JdbcTemplate, Batch Operations can be run via the batchUpdate() API.
+- 6.2. Batch Operations Using NamedParameterJdbcTemplate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> NamedParameterJdbcTemplate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JDBC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Using a List of Values in a JdbcTemplate IN Clause</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- https://www.baeldung.com/spring-jdbctemplate-in-list</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 2.2. With NamedParameterJdbcTemplate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to Specify Named Parameters Using the NamedParameterJdbcTemplate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- https://dzone.com/articles/how-to-specify-named-parameters-using-the-namedpar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>- https://www.baeldung.com/jackson-object-mapper-tutorial</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2609,7 +2666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2638,6 +2695,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -3126,20 +3186,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:F20"/>
+  <dimension ref="A4:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="8.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="68.25" style="4" customWidth="1"/>
+    <col min="6" max="6" width="57.375" style="4" customWidth="1"/>
     <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -3334,7 +3394,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
@@ -3351,7 +3411,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <v>44291</v>
       </c>
@@ -3365,7 +3425,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3382,7 +3442,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
@@ -3391,11 +3451,79 @@
       </c>
       <c r="E20" s="5" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3">
+        <v>44297</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44297</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3">
+        <v>44297</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>